<commit_message>
alınan input lar action.php 'ye gönderiliyor
</commit_message>
<xml_diff>
--- a/hello world.xlsx
+++ b/hello world.xlsx
@@ -15,15 +15,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
-  <si>
-    <t>Hello World !</t>
-  </si>
-  <si>
-    <t>Hello World-2 !</t>
-  </si>
-  <si>
-    <t>Hello World-3 !</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+  <si>
+    <t>FİYAT TEKLİFİ</t>
+  </si>
+  <si>
+    <t>FİRMA ADI</t>
+  </si>
+  <si>
+    <t>YETKİLİ ADI</t>
+  </si>
+  <si>
+    <t>TELEFON</t>
+  </si>
+  <si>
+    <t>E-POSTA</t>
+  </si>
+  <si>
+    <t>FATURA ADRESİ</t>
+  </si>
+  <si>
+    <t>VERGİ DAİRESİ/NO</t>
+  </si>
+  <si>
+    <t>S.NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ÜRÜN ADI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MODEL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ÖLÇÜ </t>
+  </si>
+  <si>
+    <t>RENK</t>
+  </si>
+  <si>
+    <t>MİKTAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BİRİM FİYATI </t>
+  </si>
+  <si>
+    <t>TUTAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GÖRSEL </t>
   </si>
 </sst>
 </file>
@@ -362,7 +401,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -370,19 +409,68 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
'B1'.$index ; cell index ine ekleme yapılıyor
</commit_message>
<xml_diff>
--- a/hello world.xlsx
+++ b/hello world.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>FİYAT TEKLİFİ</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t xml:space="preserve">GÖRSEL </t>
+  </si>
+  <si>
+    <t>ssasasasas</t>
   </si>
 </sst>
 </file>
@@ -401,7 +404,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,6 +474,11 @@
       </c>
       <c r="I10" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="B15" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
oldu sonunda;veri tabanına ekleyebiliyorum
</commit_message>
<xml_diff>
--- a/hello world.xlsx
+++ b/hello world.xlsx
@@ -401,7 +401,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,8 +473,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
-      <c r="B11"/>
+    <row r="14" spans="1:9">
+      <c r="B14"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
add query,needs table design,0
</commit_message>
<xml_diff>
--- a/hello world.xlsx
+++ b/hello world.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>FİYAT TEKLİFİ</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t xml:space="preserve">GÖRSEL </t>
+  </si>
+  <si>
+    <t>bebek bezi2</t>
   </si>
 </sst>
 </file>
@@ -474,7 +477,9 @@
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="B14"/>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
can be added more than one pic,1
</commit_message>
<xml_diff>
--- a/hello world.xlsx
+++ b/hello world.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\FormToExcel\FormToExcelPHP\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{748112C8-491A-42D7-AB93-81F62CF4A749}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>FİYAT TEKLİFİ</t>
   </si>
@@ -63,19 +68,38 @@
   </si>
   <si>
     <t xml:space="preserve">GÖRSEL </t>
+  </si>
+  <si>
+    <t>bebek bezi23</t>
+  </si>
+  <si>
+    <t>U20YELKKY.0047</t>
+  </si>
+  <si>
+    <t>bebek bezi</t>
+  </si>
+  <si>
+    <t>bebek bezi10</t>
+  </si>
+  <si>
+    <t>paid image</t>
+  </si>
+  <si>
+    <t>U20YELKKY.00478</t>
+  </si>
+  <si>
+    <t>mouse</t>
+  </si>
+  <si>
+    <t>U20YELKKYY.0048</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -86,29 +110,365 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1047750</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="952500" cy="466725"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Paid" descr="Paid">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="1500000">
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="2700000" algn="br" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="50000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1047750</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="952500" cy="466725"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Paid" descr="Paid">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="1500000">
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="2700000" algn="br" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="50000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1047750</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="952500" cy="466725"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Paid" descr="Paid">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="1500000">
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="2700000" algn="br" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="50000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1047750</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="952500" cy="466725"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Paid" descr="Paid">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="1500000">
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="2700000" algn="br" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="50000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1047750</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="952500" cy="466725"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Paid" descr="Paid">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="1500000">
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="2700000" algn="br" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="50000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1047750</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="952500" cy="466725"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Paid" descr="Paid">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="1500000">
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="2700000" algn="br" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="50000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1047750</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="952500" cy="466725"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Paid" descr="Paid">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="1500000">
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="2700000" algn="br" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="50000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -397,54 +757,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:Z11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A3:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:26">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -473,21 +830,65 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:26">
-      <c r="Z11"/>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>